<commit_message>
static routes; firewall rules
</commit_message>
<xml_diff>
--- a/docs/McSOC BOM.xlsx
+++ b/docs/McSOC BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="135">
   <si>
     <t>Server</t>
   </si>
@@ -270,6 +270,45 @@
   </si>
   <si>
     <t>IP package Integrity</t>
+  </si>
+  <si>
+    <t>nagios</t>
+  </si>
+  <si>
+    <t>Network Monitoring</t>
+  </si>
+  <si>
+    <t>Nagios</t>
+  </si>
+  <si>
+    <t>Nagios Core</t>
+  </si>
+  <si>
+    <t>https://www.nagios.org/</t>
+  </si>
+  <si>
+    <t>https://sourceforge.net/projects/nagios/files/nagios-4.x/nagios-4.2.2/nagios-4.2.2.tar.gz</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>Nagios Plugins</t>
+  </si>
+  <si>
+    <t>http://nagios-plugins.org/download/nagios-plugins-2.1.4.tar.gz</t>
+  </si>
+  <si>
+    <t>2.1.4</t>
+  </si>
+  <si>
+    <t>NagiosQL</t>
+  </si>
+  <si>
+    <t>http://sourceforge.net/projects/nagiosql/files/nagiosql/NagiosQL%203.2.0/nagiosql_320.tar.gz</t>
+  </si>
+  <si>
+    <t>3.2.0</t>
   </si>
   <si>
     <t>Perimeter</t>
@@ -395,6 +434,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -416,17 +456,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF00000A"/>
       <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -586,10 +629,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C54" activeCellId="0" sqref="C54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -652,6 +695,7 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
@@ -669,6 +713,7 @@
       <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
@@ -686,11 +731,14 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
@@ -711,6 +759,7 @@
       <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
@@ -731,6 +780,7 @@
       <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
@@ -751,6 +801,7 @@
       <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
@@ -765,6 +816,8 @@
       <c r="G9" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
@@ -779,6 +832,8 @@
       <c r="G10" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
@@ -793,6 +848,8 @@
       <c r="G11" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
@@ -807,6 +864,8 @@
       <c r="G12" s="0" t="s">
         <v>48</v>
       </c>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
@@ -821,6 +880,8 @@
       <c r="G13" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
@@ -835,6 +896,8 @@
       <c r="G14" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
@@ -957,266 +1020,341 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="5" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="B32" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>86</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>54</v>
+      <c r="E34" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>89</v>
+        <v>99</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>90</v>
+        <v>101</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="5" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>96</v>
+        <v>105</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="5" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="5" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="5" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="5" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>102</v>
+        <v>113</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="5" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>103</v>
+        <v>114</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="5" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="5" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>34</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="5" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>108</v>
+        <v>22</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="5" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>110</v>
+        <v>120</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="5" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="5" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="5" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="5" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="5" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="5" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="5" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="5" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="5" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>121</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>